<commit_message>
report and slight math fix
</commit_message>
<xml_diff>
--- a/Data Collection Project 2.xlsx
+++ b/Data Collection Project 2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t xml:space="preserve">Number of workers</t>
   </si>
@@ -46,13 +46,16 @@
     <t xml:space="preserve">index all threee at once</t>
   </si>
   <si>
+    <t xml:space="preserve">Below is the time in seconds</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indexing twelfthnight (seconds)</t>
   </si>
   <si>
-    <t xml:space="preserve">Indexing tamingoftheshrew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indexing midsummersnightsdream</t>
+    <t xml:space="preserve">Indexing tamingoftheshrew(seconds)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexing midsummersnightsdream(seconds)</t>
   </si>
 </sst>
 </file>
@@ -101,12 +104,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -135,7 +145,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -146,6 +156,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -165,10 +179,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:G19"/>
+  <dimension ref="A2:G23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -295,18 +309,23 @@
         <v>16176144036</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>4</v>
@@ -432,15 +451,13 @@
         <f aca="false">B9/1000000000</f>
         <v>24.395215589</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <f aca="false">C9/1000000000</f>
-        <v>0</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="G19" s="1" t="n">
         <f aca="false">G9/1000000000</f>
         <v>16.176144036</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>